<commit_message>
Updated Main Page & New 404
- Used animate.css for some part in index.html
- Added new 404 page
- Added new jet-estate.js under js/ folder
- Added new jquery.inview.js under js/ folder

Highlight: index.html is finished
</commit_message>
<xml_diff>
--- a/JetEstate.xlsx
+++ b/JetEstate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23835" windowHeight="9975" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23835" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Specs" sheetId="1" r:id="rId1"/>
@@ -287,10 +287,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -298,14 +306,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -631,22 +633,22 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="B8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>11</v>
+      <c r="A10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -807,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21:L21"/>
     </sheetView>
   </sheetViews>
@@ -854,284 +856,280 @@
       </c>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="5"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="F10" s="9" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="F10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="J10" s="9" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="J10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="F14" s="10" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="F14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="J14" s="10" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="J14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="10" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="F15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="J15" s="10" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="J15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="F16" s="11" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="F16" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="J16" s="11" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="J16" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="9"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="E23" s="9" t="s">
+      <c r="C23" s="11"/>
+      <c r="E23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="H23" s="9" t="s">
+      <c r="F23" s="11"/>
+      <c r="H23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="K23" s="9" t="s">
+      <c r="I23" s="11"/>
+      <c r="K23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="9"/>
+      <c r="L23" s="11"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="E25" s="13" t="s">
+      <c r="C25" s="12"/>
+      <c r="E25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="H25" s="13" t="s">
+      <c r="F25" s="12"/>
+      <c r="H25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="13"/>
-      <c r="K25" s="13" t="s">
+      <c r="I25" s="12"/>
+      <c r="K25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="L25" s="13"/>
+      <c r="L25" s="12"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="F31" s="8" t="s">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="F31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="J31" s="8" t="s">
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="J31" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
     </row>
     <row r="37" spans="2:12" ht="33.75" customHeight="1">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K23:L24"/>
-    <mergeCell ref="K25:L26"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B5:L6"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="B37:L37"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="F31:H31"/>
@@ -1142,6 +1140,11 @@
     <mergeCell ref="E25:F26"/>
     <mergeCell ref="H23:I24"/>
     <mergeCell ref="H25:I26"/>
+    <mergeCell ref="K23:L24"/>
+    <mergeCell ref="K25:L26"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B5:L6"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="J10:L13"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J15:L15"/>
@@ -1153,7 +1156,6 @@
     <mergeCell ref="F10:H13"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>